<commit_message>
Uploading AIMMS results files
</commit_message>
<xml_diff>
--- a/Data/AIMMS_results.xlsx
+++ b/Data/AIMMS_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="7">
   <si>
     <t>latitude</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>Greedy Chargers</t>
+  </si>
+  <si>
+    <t>stress</t>
   </si>
   <si>
     <t>profile</t>
@@ -389,13 +392,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E155"/>
+  <dimension ref="A1:F155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,8 +411,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -422,11 +428,14 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2">
+        <v>122.32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -439,11 +448,14 @@
       <c r="D3">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3">
+        <v>36.8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -456,11 +468,14 @@
       <c r="D4">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4">
+        <v>54.88</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -473,11 +488,14 @@
       <c r="D5">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5">
+        <v>30.4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -490,11 +508,14 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6">
+        <v>93.40000000000001</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -507,11 +528,14 @@
       <c r="D7">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7">
+        <v>123.04</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -524,11 +548,14 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8">
+        <v>71.23999999999999</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -541,11 +568,14 @@
       <c r="D9">
         <v>2</v>
       </c>
-      <c r="E9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9">
+        <v>36.68</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -558,11 +588,14 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="E10">
+        <v>88.28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -575,11 +608,14 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="E11">
+        <v>62.96</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -592,11 +628,14 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="E12">
+        <v>60.04</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -609,11 +648,14 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="E13">
+        <v>54.84</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -626,11 +668,14 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="E14">
+        <v>43.92</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -643,11 +688,14 @@
       <c r="D15">
         <v>4</v>
       </c>
-      <c r="E15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="E15">
+        <v>91.64</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -660,11 +708,14 @@
       <c r="D16">
         <v>3</v>
       </c>
-      <c r="E16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="E16">
+        <v>66.48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -677,11 +728,14 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="E17">
+        <v>120.84</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -694,11 +748,14 @@
       <c r="D18">
         <v>4</v>
       </c>
-      <c r="E18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="E18">
+        <v>17.04</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -711,11 +768,14 @@
       <c r="D19">
         <v>3</v>
       </c>
-      <c r="E19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="E19">
+        <v>102.08</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -728,11 +788,14 @@
       <c r="D20">
         <v>8</v>
       </c>
-      <c r="E20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="E20">
+        <v>113.8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -745,11 +808,14 @@
       <c r="D21">
         <v>2</v>
       </c>
-      <c r="E21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="E21">
+        <v>83.12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -762,11 +828,14 @@
       <c r="D22">
         <v>2</v>
       </c>
-      <c r="E22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="E22">
+        <v>96.36</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -779,11 +848,14 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="E23">
+        <v>50.84</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -796,11 +868,14 @@
       <c r="D24">
         <v>2</v>
       </c>
-      <c r="E24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="E24">
+        <v>20.84</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -813,11 +888,14 @@
       <c r="D25">
         <v>2</v>
       </c>
-      <c r="E25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="E25">
+        <v>8.08</v>
+      </c>
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -830,11 +908,14 @@
       <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="E26">
+        <v>46.28</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -847,11 +928,14 @@
       <c r="D27">
         <v>3</v>
       </c>
-      <c r="E27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="E27">
+        <v>78.08</v>
+      </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -864,11 +948,14 @@
       <c r="D28">
         <v>5</v>
       </c>
-      <c r="E28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="E28">
+        <v>55.84</v>
+      </c>
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -881,11 +968,14 @@
       <c r="D29">
         <v>4</v>
       </c>
-      <c r="E29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="E29">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="F29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -898,11 +988,14 @@
       <c r="D30">
         <v>3</v>
       </c>
-      <c r="E30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="E30">
+        <v>19.6</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -915,11 +1008,14 @@
       <c r="D31">
         <v>8</v>
       </c>
-      <c r="E31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="E31">
+        <v>133.68</v>
+      </c>
+      <c r="F31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -932,11 +1028,14 @@
       <c r="D32">
         <v>2</v>
       </c>
-      <c r="E32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="E32">
+        <v>44.4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -949,11 +1048,14 @@
       <c r="D33">
         <v>1</v>
       </c>
-      <c r="E33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="E33">
+        <v>24.76</v>
+      </c>
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -966,11 +1068,14 @@
       <c r="D34">
         <v>2</v>
       </c>
-      <c r="E34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="E34">
+        <v>79.72</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -983,11 +1088,14 @@
       <c r="D35">
         <v>6</v>
       </c>
-      <c r="E35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="E35">
+        <v>87.2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1000,11 +1108,14 @@
       <c r="D36">
         <v>5</v>
       </c>
-      <c r="E36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="E36">
+        <v>70.12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1017,11 +1128,14 @@
       <c r="D37">
         <v>2</v>
       </c>
-      <c r="E37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="E37">
+        <v>25</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1034,11 +1148,14 @@
       <c r="D38">
         <v>1</v>
       </c>
-      <c r="E38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="E38">
+        <v>92</v>
+      </c>
+      <c r="F38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1051,11 +1168,14 @@
       <c r="D39">
         <v>1</v>
       </c>
-      <c r="E39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="E39">
+        <v>66.68000000000001</v>
+      </c>
+      <c r="F39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1068,11 +1188,14 @@
       <c r="D40">
         <v>8</v>
       </c>
-      <c r="E40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="E40">
+        <v>99.88</v>
+      </c>
+      <c r="F40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1085,11 +1208,14 @@
       <c r="D41">
         <v>1</v>
       </c>
-      <c r="E41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="E41">
+        <v>29.72</v>
+      </c>
+      <c r="F41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1102,11 +1228,14 @@
       <c r="D42">
         <v>2</v>
       </c>
-      <c r="E42" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="E42">
+        <v>71.08</v>
+      </c>
+      <c r="F42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1119,11 +1248,14 @@
       <c r="D43">
         <v>3</v>
       </c>
-      <c r="E43" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="E43">
+        <v>70.92</v>
+      </c>
+      <c r="F43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1136,11 +1268,14 @@
       <c r="D44">
         <v>8</v>
       </c>
-      <c r="E44" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="E44">
+        <v>153.92</v>
+      </c>
+      <c r="F44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1153,11 +1288,14 @@
       <c r="D45">
         <v>2</v>
       </c>
-      <c r="E45" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="E45">
+        <v>16.32</v>
+      </c>
+      <c r="F45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1170,11 +1308,14 @@
       <c r="D46">
         <v>5</v>
       </c>
-      <c r="E46" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="E46">
+        <v>58.68</v>
+      </c>
+      <c r="F46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1187,11 +1328,14 @@
       <c r="D47">
         <v>3</v>
       </c>
-      <c r="E47" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="E47">
+        <v>32.96</v>
+      </c>
+      <c r="F47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1204,11 +1348,14 @@
       <c r="D48">
         <v>2</v>
       </c>
-      <c r="E48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="E48">
+        <v>30.16</v>
+      </c>
+      <c r="F48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1221,11 +1368,14 @@
       <c r="D49">
         <v>5</v>
       </c>
-      <c r="E49" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="E49">
+        <v>63.52</v>
+      </c>
+      <c r="F49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1238,11 +1388,14 @@
       <c r="D50">
         <v>8</v>
       </c>
-      <c r="E50" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="E50">
+        <v>68.31999999999999</v>
+      </c>
+      <c r="F50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1255,11 +1408,14 @@
       <c r="D51">
         <v>8</v>
       </c>
-      <c r="E51" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="E51">
+        <v>79.12</v>
+      </c>
+      <c r="F51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1272,11 +1428,14 @@
       <c r="D52">
         <v>2</v>
       </c>
-      <c r="E52" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="E52">
+        <v>8.16</v>
+      </c>
+      <c r="F52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1289,11 +1448,14 @@
       <c r="D53">
         <v>3</v>
       </c>
-      <c r="E53" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="E53">
+        <v>28.88</v>
+      </c>
+      <c r="F53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1306,11 +1468,14 @@
       <c r="D54">
         <v>3</v>
       </c>
-      <c r="E54" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="E54">
+        <v>129.6</v>
+      </c>
+      <c r="F54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1323,11 +1488,14 @@
       <c r="D55">
         <v>8</v>
       </c>
-      <c r="E55" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="E55">
+        <v>76.23999999999999</v>
+      </c>
+      <c r="F55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1340,11 +1508,14 @@
       <c r="D56">
         <v>2</v>
       </c>
-      <c r="E56" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="E56">
+        <v>123.8</v>
+      </c>
+      <c r="F56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1357,11 +1528,14 @@
       <c r="D57">
         <v>3</v>
       </c>
-      <c r="E57" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="E57">
+        <v>16.92</v>
+      </c>
+      <c r="F57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1374,11 +1548,14 @@
       <c r="D58">
         <v>2</v>
       </c>
-      <c r="E58" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="E58">
+        <v>55.48</v>
+      </c>
+      <c r="F58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1391,11 +1568,14 @@
       <c r="D59">
         <v>2</v>
       </c>
-      <c r="E59" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="E59">
+        <v>38.96</v>
+      </c>
+      <c r="F59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1408,11 +1588,14 @@
       <c r="D60">
         <v>7</v>
       </c>
-      <c r="E60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="E60">
+        <v>66.44</v>
+      </c>
+      <c r="F60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1425,11 +1608,14 @@
       <c r="D61">
         <v>8</v>
       </c>
-      <c r="E61" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="E61">
+        <v>87.95999999999999</v>
+      </c>
+      <c r="F61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -1442,11 +1628,14 @@
       <c r="D62">
         <v>1</v>
       </c>
-      <c r="E62" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="E62">
+        <v>33.84</v>
+      </c>
+      <c r="F62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -1459,11 +1648,14 @@
       <c r="D63">
         <v>1</v>
       </c>
-      <c r="E63" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="E63">
+        <v>41.96</v>
+      </c>
+      <c r="F63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -1476,11 +1668,14 @@
       <c r="D64">
         <v>1</v>
       </c>
-      <c r="E64" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="E64">
+        <v>29.04</v>
+      </c>
+      <c r="F64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -1493,11 +1688,14 @@
       <c r="D65">
         <v>3</v>
       </c>
-      <c r="E65" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="E65">
+        <v>44.96</v>
+      </c>
+      <c r="F65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -1510,11 +1708,14 @@
       <c r="D66">
         <v>2</v>
       </c>
-      <c r="E66" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="E66">
+        <v>62.2</v>
+      </c>
+      <c r="F66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -1527,11 +1728,14 @@
       <c r="D67">
         <v>3</v>
       </c>
-      <c r="E67" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="E67">
+        <v>147.68</v>
+      </c>
+      <c r="F67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -1544,11 +1748,14 @@
       <c r="D68">
         <v>8</v>
       </c>
-      <c r="E68" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="E68">
+        <v>196.12</v>
+      </c>
+      <c r="F68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -1561,11 +1768,14 @@
       <c r="D69">
         <v>1</v>
       </c>
-      <c r="E69" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="E69">
+        <v>29.08</v>
+      </c>
+      <c r="F69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -1578,11 +1788,14 @@
       <c r="D70">
         <v>8</v>
       </c>
-      <c r="E70" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="E70">
+        <v>55.52</v>
+      </c>
+      <c r="F70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -1595,11 +1808,14 @@
       <c r="D71">
         <v>3</v>
       </c>
-      <c r="E71" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="E71">
+        <v>36.04</v>
+      </c>
+      <c r="F71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -1612,11 +1828,14 @@
       <c r="D72">
         <v>4</v>
       </c>
-      <c r="E72" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="E72">
+        <v>24.96</v>
+      </c>
+      <c r="F72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -1629,11 +1848,14 @@
       <c r="D73">
         <v>4</v>
       </c>
-      <c r="E73" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="E73">
+        <v>79.36</v>
+      </c>
+      <c r="F73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -1646,11 +1868,14 @@
       <c r="D74">
         <v>5</v>
       </c>
-      <c r="E74" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="E74">
+        <v>105.64</v>
+      </c>
+      <c r="F74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -1663,11 +1888,14 @@
       <c r="D75">
         <v>2</v>
       </c>
-      <c r="E75" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="E75">
+        <v>21.48</v>
+      </c>
+      <c r="F75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -1680,11 +1908,14 @@
       <c r="D76">
         <v>5</v>
       </c>
-      <c r="E76" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="E76">
+        <v>29.32</v>
+      </c>
+      <c r="F76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -1697,11 +1928,14 @@
       <c r="D77">
         <v>8</v>
       </c>
-      <c r="E77" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="E77">
+        <v>99.40000000000001</v>
+      </c>
+      <c r="F77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -1714,11 +1948,14 @@
       <c r="D78">
         <v>8</v>
       </c>
-      <c r="E78" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="E78">
+        <v>65.40000000000001</v>
+      </c>
+      <c r="F78" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -1731,11 +1968,14 @@
       <c r="D79">
         <v>6</v>
       </c>
-      <c r="E79" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="E79">
+        <v>56.92</v>
+      </c>
+      <c r="F79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -1748,11 +1988,14 @@
       <c r="D80">
         <v>8</v>
       </c>
-      <c r="E80" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="E80">
+        <v>197</v>
+      </c>
+      <c r="F80" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -1765,11 +2008,14 @@
       <c r="D81">
         <v>4</v>
       </c>
-      <c r="E81" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="E81">
+        <v>33.76</v>
+      </c>
+      <c r="F81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -1782,11 +2028,14 @@
       <c r="D82">
         <v>3</v>
       </c>
-      <c r="E82" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="E82">
+        <v>49</v>
+      </c>
+      <c r="F82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -1799,11 +2048,14 @@
       <c r="D83">
         <v>5</v>
       </c>
-      <c r="E83" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="E83">
+        <v>34.36</v>
+      </c>
+      <c r="F83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -1816,11 +2068,14 @@
       <c r="D84">
         <v>3</v>
       </c>
-      <c r="E84" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="E84">
+        <v>12.72</v>
+      </c>
+      <c r="F84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -1833,11 +2088,14 @@
       <c r="D85">
         <v>5</v>
       </c>
-      <c r="E85" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="E85">
+        <v>42</v>
+      </c>
+      <c r="F85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -1850,11 +2108,14 @@
       <c r="D86">
         <v>8</v>
       </c>
-      <c r="E86" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="E86">
+        <v>63.12</v>
+      </c>
+      <c r="F86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -1867,11 +2128,14 @@
       <c r="D87">
         <v>1</v>
       </c>
-      <c r="E87" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="E87">
+        <v>63.12</v>
+      </c>
+      <c r="F87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -1884,11 +2148,14 @@
       <c r="D88">
         <v>2</v>
       </c>
-      <c r="E88" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="E88">
+        <v>25.52</v>
+      </c>
+      <c r="F88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -1901,11 +2168,14 @@
       <c r="D89">
         <v>8</v>
       </c>
-      <c r="E89" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="E89">
+        <v>57.44</v>
+      </c>
+      <c r="F89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -1918,11 +2188,14 @@
       <c r="D90">
         <v>8</v>
       </c>
-      <c r="E90" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="E90">
+        <v>196.16</v>
+      </c>
+      <c r="F90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -1935,11 +2208,14 @@
       <c r="D91">
         <v>2</v>
       </c>
-      <c r="E91" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="E91">
+        <v>21.28</v>
+      </c>
+      <c r="F91" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -1952,11 +2228,14 @@
       <c r="D92">
         <v>2</v>
       </c>
-      <c r="E92" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="E92">
+        <v>55.08</v>
+      </c>
+      <c r="F92" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -1969,11 +2248,14 @@
       <c r="D93">
         <v>1</v>
       </c>
-      <c r="E93" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="E93">
+        <v>10.6</v>
+      </c>
+      <c r="F93" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -1986,11 +2268,14 @@
       <c r="D94">
         <v>1</v>
       </c>
-      <c r="E94" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="E94">
+        <v>45.96</v>
+      </c>
+      <c r="F94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2003,11 +2288,14 @@
       <c r="D95">
         <v>8</v>
       </c>
-      <c r="E95" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="E95">
+        <v>71.16</v>
+      </c>
+      <c r="F95" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -2020,11 +2308,14 @@
       <c r="D96">
         <v>4</v>
       </c>
-      <c r="E96" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="E96">
+        <v>25.36</v>
+      </c>
+      <c r="F96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -2037,11 +2328,14 @@
       <c r="D97">
         <v>3</v>
       </c>
-      <c r="E97" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="E97">
+        <v>65.36</v>
+      </c>
+      <c r="F97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -2054,11 +2348,14 @@
       <c r="D98">
         <v>3</v>
       </c>
-      <c r="E98" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="E98">
+        <v>33.32</v>
+      </c>
+      <c r="F98" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -2071,11 +2368,14 @@
       <c r="D99">
         <v>6</v>
       </c>
-      <c r="E99" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="E99">
+        <v>39.2</v>
+      </c>
+      <c r="F99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -2088,11 +2388,14 @@
       <c r="D100">
         <v>8</v>
       </c>
-      <c r="E100" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5">
+      <c r="E100">
+        <v>92.52</v>
+      </c>
+      <c r="F100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -2105,11 +2408,14 @@
       <c r="D101">
         <v>3</v>
       </c>
-      <c r="E101" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="E101">
+        <v>80.56</v>
+      </c>
+      <c r="F101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -2122,11 +2428,14 @@
       <c r="D102">
         <v>1</v>
       </c>
-      <c r="E102" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="E102">
+        <v>59.2</v>
+      </c>
+      <c r="F102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -2139,11 +2448,14 @@
       <c r="D103">
         <v>6</v>
       </c>
-      <c r="E103" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="E103">
+        <v>33.08</v>
+      </c>
+      <c r="F103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -2156,11 +2468,14 @@
       <c r="D104">
         <v>7</v>
       </c>
-      <c r="E104" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="E104">
+        <v>34.12</v>
+      </c>
+      <c r="F104" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -2173,11 +2488,14 @@
       <c r="D105">
         <v>2</v>
       </c>
-      <c r="E105" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="E105">
+        <v>111.04</v>
+      </c>
+      <c r="F105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -2190,11 +2508,14 @@
       <c r="D106">
         <v>8</v>
       </c>
-      <c r="E106" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="E106">
+        <v>118.76</v>
+      </c>
+      <c r="F106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -2207,11 +2528,14 @@
       <c r="D107">
         <v>8</v>
       </c>
-      <c r="E107" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="E107">
+        <v>67.23999999999999</v>
+      </c>
+      <c r="F107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -2224,11 +2548,14 @@
       <c r="D108">
         <v>8</v>
       </c>
-      <c r="E108" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="E108">
+        <v>86.56</v>
+      </c>
+      <c r="F108" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -2241,11 +2568,14 @@
       <c r="D109">
         <v>8</v>
       </c>
-      <c r="E109" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="E109">
+        <v>108.8</v>
+      </c>
+      <c r="F109" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -2258,11 +2588,14 @@
       <c r="D110">
         <v>2</v>
       </c>
-      <c r="E110" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="E110">
+        <v>20.44</v>
+      </c>
+      <c r="F110" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -2275,11 +2608,14 @@
       <c r="D111">
         <v>2</v>
       </c>
-      <c r="E111" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
+      <c r="E111">
+        <v>100.2</v>
+      </c>
+      <c r="F111" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -2292,11 +2628,14 @@
       <c r="D112">
         <v>6</v>
       </c>
-      <c r="E112" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5">
+      <c r="E112">
+        <v>100.8</v>
+      </c>
+      <c r="F112" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -2309,11 +2648,14 @@
       <c r="D113">
         <v>6</v>
       </c>
-      <c r="E113" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5">
+      <c r="E113">
+        <v>33.4</v>
+      </c>
+      <c r="F113" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -2326,11 +2668,14 @@
       <c r="D114">
         <v>8</v>
       </c>
-      <c r="E114" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5">
+      <c r="E114">
+        <v>148.44</v>
+      </c>
+      <c r="F114" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -2343,11 +2688,14 @@
       <c r="D115">
         <v>8</v>
       </c>
-      <c r="E115" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5">
+      <c r="E115">
+        <v>120.56</v>
+      </c>
+      <c r="F115" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -2360,11 +2708,14 @@
       <c r="D116">
         <v>8</v>
       </c>
-      <c r="E116" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5">
+      <c r="E116">
+        <v>102.08</v>
+      </c>
+      <c r="F116" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -2377,11 +2728,14 @@
       <c r="D117">
         <v>8</v>
       </c>
-      <c r="E117" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5">
+      <c r="E117">
+        <v>53.08</v>
+      </c>
+      <c r="F117" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -2394,11 +2748,14 @@
       <c r="D118">
         <v>8</v>
       </c>
-      <c r="E118" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5">
+      <c r="E118">
+        <v>75.52</v>
+      </c>
+      <c r="F118" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -2411,11 +2768,14 @@
       <c r="D119">
         <v>8</v>
       </c>
-      <c r="E119" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5">
+      <c r="E119">
+        <v>193</v>
+      </c>
+      <c r="F119" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -2428,11 +2788,14 @@
       <c r="D120">
         <v>1</v>
       </c>
-      <c r="E120" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5">
+      <c r="E120">
+        <v>24</v>
+      </c>
+      <c r="F120" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -2445,11 +2808,14 @@
       <c r="D121">
         <v>5</v>
       </c>
-      <c r="E121" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5">
+      <c r="E121">
+        <v>49.8</v>
+      </c>
+      <c r="F121" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -2462,11 +2828,14 @@
       <c r="D122">
         <v>3</v>
       </c>
-      <c r="E122" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5">
+      <c r="E122">
+        <v>134.48</v>
+      </c>
+      <c r="F122" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -2479,11 +2848,14 @@
       <c r="D123">
         <v>7</v>
       </c>
-      <c r="E123" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5">
+      <c r="E123">
+        <v>71.2</v>
+      </c>
+      <c r="F123" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -2496,11 +2868,14 @@
       <c r="D124">
         <v>5</v>
       </c>
-      <c r="E124" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5">
+      <c r="E124">
+        <v>41.56</v>
+      </c>
+      <c r="F124" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -2513,11 +2888,14 @@
       <c r="D125">
         <v>5</v>
       </c>
-      <c r="E125" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5">
+      <c r="E125">
+        <v>46.68</v>
+      </c>
+      <c r="F125" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -2530,11 +2908,14 @@
       <c r="D126">
         <v>3</v>
       </c>
-      <c r="E126" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5">
+      <c r="E126">
+        <v>21.24</v>
+      </c>
+      <c r="F126" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -2547,11 +2928,14 @@
       <c r="D127">
         <v>6</v>
       </c>
-      <c r="E127" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5">
+      <c r="E127">
+        <v>177.84</v>
+      </c>
+      <c r="F127" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -2564,11 +2948,14 @@
       <c r="D128">
         <v>8</v>
       </c>
-      <c r="E128" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5">
+      <c r="E128">
+        <v>75.2</v>
+      </c>
+      <c r="F128" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -2581,11 +2968,14 @@
       <c r="D129">
         <v>8</v>
       </c>
-      <c r="E129" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5">
+      <c r="E129">
+        <v>113.64</v>
+      </c>
+      <c r="F129" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -2598,11 +2988,14 @@
       <c r="D130">
         <v>7</v>
       </c>
-      <c r="E130" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5">
+      <c r="E130">
+        <v>105.6</v>
+      </c>
+      <c r="F130" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -2615,11 +3008,14 @@
       <c r="D131">
         <v>8</v>
       </c>
-      <c r="E131" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5">
+      <c r="E131">
+        <v>100.52</v>
+      </c>
+      <c r="F131" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -2632,11 +3028,14 @@
       <c r="D132">
         <v>8</v>
       </c>
-      <c r="E132" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5">
+      <c r="E132">
+        <v>99.56</v>
+      </c>
+      <c r="F132" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -2649,11 +3048,14 @@
       <c r="D133">
         <v>8</v>
       </c>
-      <c r="E133" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="E133">
+        <v>83.28</v>
+      </c>
+      <c r="F133" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -2666,11 +3068,14 @@
       <c r="D134">
         <v>3</v>
       </c>
-      <c r="E134" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5">
+      <c r="E134">
+        <v>32.24</v>
+      </c>
+      <c r="F134" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -2683,11 +3088,14 @@
       <c r="D135">
         <v>8</v>
       </c>
-      <c r="E135" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5">
+      <c r="E135">
+        <v>65.92</v>
+      </c>
+      <c r="F135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -2700,11 +3108,14 @@
       <c r="D136">
         <v>5</v>
       </c>
-      <c r="E136" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5">
+      <c r="E136">
+        <v>26.24</v>
+      </c>
+      <c r="F136" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -2717,11 +3128,14 @@
       <c r="D137">
         <v>2</v>
       </c>
-      <c r="E137" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5">
+      <c r="E137">
+        <v>12.6</v>
+      </c>
+      <c r="F137" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -2734,11 +3148,14 @@
       <c r="D138">
         <v>3</v>
       </c>
-      <c r="E138" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5">
+      <c r="E138">
+        <v>29.64</v>
+      </c>
+      <c r="F138" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -2751,11 +3168,14 @@
       <c r="D139">
         <v>8</v>
       </c>
-      <c r="E139" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5">
+      <c r="E139">
+        <v>99.40000000000001</v>
+      </c>
+      <c r="F139" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -2768,11 +3188,14 @@
       <c r="D140">
         <v>6</v>
       </c>
-      <c r="E140" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5">
+      <c r="E140">
+        <v>50.32</v>
+      </c>
+      <c r="F140" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -2785,11 +3208,14 @@
       <c r="D141">
         <v>6</v>
       </c>
-      <c r="E141" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5">
+      <c r="E141">
+        <v>42.44</v>
+      </c>
+      <c r="F141" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -2802,11 +3228,14 @@
       <c r="D142">
         <v>4</v>
       </c>
-      <c r="E142" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5">
+      <c r="E142">
+        <v>101.32</v>
+      </c>
+      <c r="F142" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -2819,11 +3248,14 @@
       <c r="D143">
         <v>5</v>
       </c>
-      <c r="E143" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5">
+      <c r="E143">
+        <v>37.4</v>
+      </c>
+      <c r="F143" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -2836,11 +3268,14 @@
       <c r="D144">
         <v>3</v>
       </c>
-      <c r="E144" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5">
+      <c r="E144">
+        <v>44.28</v>
+      </c>
+      <c r="F144" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -2853,11 +3288,14 @@
       <c r="D145">
         <v>3</v>
       </c>
-      <c r="E145" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5">
+      <c r="E145">
+        <v>8.44</v>
+      </c>
+      <c r="F145" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -2870,11 +3308,14 @@
       <c r="D146">
         <v>8</v>
       </c>
-      <c r="E146" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5">
+      <c r="E146">
+        <v>168.6</v>
+      </c>
+      <c r="F146" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -2887,11 +3328,14 @@
       <c r="D147">
         <v>5</v>
       </c>
-      <c r="E147" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5">
+      <c r="E147">
+        <v>38.12</v>
+      </c>
+      <c r="F147" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -2904,11 +3348,14 @@
       <c r="D148">
         <v>3</v>
       </c>
-      <c r="E148" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5">
+      <c r="E148">
+        <v>67.8</v>
+      </c>
+      <c r="F148" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -2921,11 +3368,14 @@
       <c r="D149">
         <v>8</v>
       </c>
-      <c r="E149" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5">
+      <c r="E149">
+        <v>169</v>
+      </c>
+      <c r="F149" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -2938,11 +3388,14 @@
       <c r="D150">
         <v>6</v>
       </c>
-      <c r="E150" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5">
+      <c r="E150">
+        <v>45.04</v>
+      </c>
+      <c r="F150" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -2955,11 +3408,14 @@
       <c r="D151">
         <v>5</v>
       </c>
-      <c r="E151" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5">
+      <c r="E151">
+        <v>57.56</v>
+      </c>
+      <c r="F151" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -2972,11 +3428,14 @@
       <c r="D152">
         <v>5</v>
       </c>
-      <c r="E152" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5">
+      <c r="E152">
+        <v>29.12</v>
+      </c>
+      <c r="F152" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -2989,11 +3448,14 @@
       <c r="D153">
         <v>2</v>
       </c>
-      <c r="E153" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5">
+      <c r="E153">
+        <v>16.4</v>
+      </c>
+      <c r="F153" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -3006,11 +3468,14 @@
       <c r="D154">
         <v>3</v>
       </c>
-      <c r="E154" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5">
+      <c r="E154">
+        <v>29.32</v>
+      </c>
+      <c r="F154" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -3023,8 +3488,11 @@
       <c r="D155">
         <v>8</v>
       </c>
-      <c r="E155" t="s">
-        <v>4</v>
+      <c r="E155">
+        <v>64.44</v>
+      </c>
+      <c r="F155" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>